<commit_message>
Added x86 Intel Core(TM) i7-2620M CPU @ 2.7GHz run 2 test.
Added Linux Code.
</commit_message>
<xml_diff>
--- a/Results/Benchmark_April_6th _no_i.xlsx
+++ b/Results/Benchmark_April_6th _no_i.xlsx
@@ -12,14 +12,15 @@
     <sheet name="TI DSP 4 Cores" sheetId="3" r:id="rId3"/>
     <sheet name="TI DSP 7 Cores" sheetId="4" r:id="rId4"/>
     <sheet name="TI DSP 8 Cores" sheetId="5" r:id="rId5"/>
-    <sheet name="Mac i7 x86 @2.7GHz" sheetId="2" r:id="rId6"/>
+    <sheet name="Mac i7-2620M x86 @2.7GHz run 1" sheetId="2" r:id="rId6"/>
+    <sheet name="Mac i7-2620M x86 @2.7GHz run 2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="138">
   <si>
     <t>1MB</t>
   </si>
@@ -795,32 +796,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -831,6 +814,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -839,6 +831,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1179,29 +1180,29 @@
       <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
       <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
     </row>
     <row r="2" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D2" s="14"/>
@@ -1397,69 +1398,69 @@
       <c r="E7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45" t="s">
+      <c r="G7" s="47"/>
+      <c r="H7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45" t="s">
+      <c r="I7" s="47"/>
+      <c r="J7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45" t="s">
+      <c r="K7" s="47"/>
+      <c r="L7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="45"/>
+      <c r="M7" s="47"/>
       <c r="O7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="45" t="s">
+      <c r="P7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45" t="s">
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45" t="s">
+      <c r="S7" s="47"/>
+      <c r="T7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45" t="s">
+      <c r="U7" s="47"/>
+      <c r="V7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="W7" s="45"/>
+      <c r="W7" s="47"/>
     </row>
     <row r="8" spans="4:23" x14ac:dyDescent="0.25">
       <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
       <c r="O8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P8" s="41" t="s">
+      <c r="P8" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
     </row>
     <row r="9" spans="4:23" ht="30" x14ac:dyDescent="0.25">
       <c r="E9" s="13" t="s">
@@ -2594,11 +2595,11 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
       <c r="E25" s="35" t="s">
         <v>31</v>
       </c>
@@ -2671,9 +2672,9 @@
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
       <c r="E26" s="3"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
@@ -2694,10 +2695,10 @@
       <c r="W26" s="28"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="51"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="E27" s="43" t="s">
+      <c r="A27" s="45"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="E27" s="48" t="s">
         <v>43</v>
       </c>
       <c r="F27" s="27"/>
@@ -2728,7 +2729,7 @@
       <c r="C28" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="44"/>
+      <c r="E28" s="49"/>
       <c r="F28" s="27"/>
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
@@ -2761,22 +2762,22 @@
       <c r="E29" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F29" s="45" t="s">
+      <c r="F29" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45" t="s">
+      <c r="G29" s="47"/>
+      <c r="H29" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45" t="s">
+      <c r="I29" s="47"/>
+      <c r="J29" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45" t="s">
+      <c r="K29" s="47"/>
+      <c r="L29" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M29" s="45"/>
+      <c r="M29" s="47"/>
       <c r="O29" s="3"/>
       <c r="P29" s="28"/>
       <c r="Q29" s="28"/>
@@ -2801,16 +2802,16 @@
       <c r="E30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="41" t="s">
+      <c r="F30" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
     </row>
     <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -2850,17 +2851,17 @@
       <c r="M31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O31" s="53" t="s">
+      <c r="O31" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="P31" s="54"/>
-      <c r="Q31" s="54"/>
-      <c r="R31" s="54"/>
-      <c r="S31" s="54"/>
-      <c r="T31" s="54"/>
-      <c r="U31" s="54"/>
-      <c r="V31" s="54"/>
-      <c r="W31" s="55"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="51"/>
+      <c r="V31" s="51"/>
+      <c r="W31" s="52"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -3499,62 +3500,62 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E48" s="50" t="s">
+      <c r="E48" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
-      <c r="K48" s="50"/>
-      <c r="L48" s="50"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="44"/>
       <c r="M48" s="30"/>
       <c r="N48" s="31"/>
     </row>
     <row r="50" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E50" s="43" t="s">
+      <c r="E50" s="48" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="51" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E51" s="44"/>
+      <c r="E51" s="49"/>
     </row>
     <row r="52" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E52" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F52" s="45" t="s">
+      <c r="F52" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G52" s="45"/>
-      <c r="H52" s="45" t="s">
+      <c r="G52" s="47"/>
+      <c r="H52" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I52" s="45"/>
-      <c r="J52" s="45" t="s">
+      <c r="I52" s="47"/>
+      <c r="J52" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K52" s="45"/>
-      <c r="L52" s="45" t="s">
+      <c r="K52" s="47"/>
+      <c r="L52" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M52" s="45"/>
+      <c r="M52" s="47"/>
     </row>
     <row r="53" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E53" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="41" t="s">
+      <c r="F53" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="42"/>
-      <c r="J53" s="42"/>
-      <c r="K53" s="42"/>
-      <c r="L53" s="42"/>
-      <c r="M53" s="42"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="43"/>
+      <c r="M53" s="43"/>
     </row>
     <row r="54" spans="5:13" ht="30" x14ac:dyDescent="0.25">
       <c r="E54" s="13" t="s">
@@ -4174,7 +4175,7 @@
       </c>
     </row>
     <row r="72" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D72" s="49" t="s">
+      <c r="D72" s="41" t="s">
         <v>100</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -4194,7 +4195,7 @@
       </c>
     </row>
     <row r="73" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D73" s="49"/>
+      <c r="D73" s="41"/>
       <c r="E73" s="1" t="s">
         <v>108</v>
       </c>
@@ -4723,6 +4724,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="F53:M53"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="P8:W8"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="L7:M7"/>
     <mergeCell ref="D72:D73"/>
     <mergeCell ref="F30:M30"/>
     <mergeCell ref="E48:L48"/>
@@ -4739,20 +4754,6 @@
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="P8:W8"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="F53:M53"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="L52:M52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4799,29 +4800,29 @@
       <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
       <c r="O1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="46" t="s">
+      <c r="P1" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
     </row>
     <row r="2" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D2" s="40"/>
@@ -5017,69 +5018,69 @@
       <c r="E7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45" t="s">
+      <c r="G7" s="47"/>
+      <c r="H7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45" t="s">
+      <c r="I7" s="47"/>
+      <c r="J7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45" t="s">
+      <c r="K7" s="47"/>
+      <c r="L7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="45"/>
+      <c r="M7" s="47"/>
       <c r="O7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="45" t="s">
+      <c r="P7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45" t="s">
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45" t="s">
+      <c r="S7" s="47"/>
+      <c r="T7" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45" t="s">
+      <c r="U7" s="47"/>
+      <c r="V7" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="W7" s="45"/>
+      <c r="W7" s="47"/>
     </row>
     <row r="8" spans="4:23" x14ac:dyDescent="0.25">
       <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
       <c r="O8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P8" s="41" t="s">
+      <c r="P8" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="V8" s="42"/>
-      <c r="W8" s="42"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
     </row>
     <row r="9" spans="4:23" ht="30" x14ac:dyDescent="0.25">
       <c r="E9" s="13" t="s">
@@ -6214,11 +6215,11 @@
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
       <c r="E25" s="35" t="s">
         <v>31</v>
       </c>
@@ -6291,9 +6292,9 @@
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="45"/>
+      <c r="C26" s="45"/>
       <c r="E26" s="3"/>
       <c r="F26" s="27"/>
       <c r="G26" s="27"/>
@@ -6314,10 +6315,10 @@
       <c r="W26" s="28"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="51"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="E27" s="43" t="s">
+      <c r="A27" s="45"/>
+      <c r="B27" s="45"/>
+      <c r="C27" s="45"/>
+      <c r="E27" s="48" t="s">
         <v>43</v>
       </c>
       <c r="F27" s="27"/>
@@ -6348,7 +6349,7 @@
       <c r="C28" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="44"/>
+      <c r="E28" s="49"/>
       <c r="F28" s="27"/>
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
@@ -6381,22 +6382,22 @@
       <c r="E29" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F29" s="45" t="s">
+      <c r="F29" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45" t="s">
+      <c r="G29" s="47"/>
+      <c r="H29" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45" t="s">
+      <c r="I29" s="47"/>
+      <c r="J29" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45" t="s">
+      <c r="K29" s="47"/>
+      <c r="L29" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M29" s="45"/>
+      <c r="M29" s="47"/>
       <c r="O29" s="3"/>
       <c r="P29" s="28"/>
       <c r="Q29" s="28"/>
@@ -6421,16 +6422,16 @@
       <c r="E30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="41" t="s">
+      <c r="F30" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="42"/>
-      <c r="M30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
     </row>
     <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
@@ -6470,17 +6471,17 @@
       <c r="M31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O31" s="53" t="s">
+      <c r="O31" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="P31" s="54"/>
-      <c r="Q31" s="54"/>
-      <c r="R31" s="54"/>
-      <c r="S31" s="54"/>
-      <c r="T31" s="54"/>
-      <c r="U31" s="54"/>
-      <c r="V31" s="54"/>
-      <c r="W31" s="55"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
+      <c r="T31" s="51"/>
+      <c r="U31" s="51"/>
+      <c r="V31" s="51"/>
+      <c r="W31" s="52"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
@@ -7119,62 +7120,62 @@
       </c>
     </row>
     <row r="48" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E48" s="50" t="s">
+      <c r="E48" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
-      <c r="K48" s="50"/>
-      <c r="L48" s="50"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="44"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="44"/>
+      <c r="L48" s="44"/>
       <c r="M48" s="30"/>
       <c r="N48" s="31"/>
     </row>
     <row r="50" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E50" s="43" t="s">
+      <c r="E50" s="48" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="51" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E51" s="44"/>
+      <c r="E51" s="49"/>
     </row>
     <row r="52" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E52" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F52" s="45" t="s">
+      <c r="F52" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G52" s="45"/>
-      <c r="H52" s="45" t="s">
+      <c r="G52" s="47"/>
+      <c r="H52" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I52" s="45"/>
-      <c r="J52" s="45" t="s">
+      <c r="I52" s="47"/>
+      <c r="J52" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K52" s="45"/>
-      <c r="L52" s="45" t="s">
+      <c r="K52" s="47"/>
+      <c r="L52" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M52" s="45"/>
+      <c r="M52" s="47"/>
     </row>
     <row r="53" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E53" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="41" t="s">
+      <c r="F53" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
-      <c r="I53" s="42"/>
-      <c r="J53" s="42"/>
-      <c r="K53" s="42"/>
-      <c r="L53" s="42"/>
-      <c r="M53" s="42"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="43"/>
+      <c r="M53" s="43"/>
     </row>
     <row r="54" spans="5:13" ht="30" x14ac:dyDescent="0.25">
       <c r="E54" s="13" t="s">
@@ -7794,7 +7795,7 @@
       </c>
     </row>
     <row r="72" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D72" s="49" t="s">
+      <c r="D72" s="41" t="s">
         <v>100</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -7814,7 +7815,7 @@
       </c>
     </row>
     <row r="73" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D73" s="49"/>
+      <c r="D73" s="41"/>
       <c r="E73" s="1" t="s">
         <v>108</v>
       </c>
@@ -8335,18 +8336,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="A25:C27"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="F53:M53"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E48:L48"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="L52:M52"/>
     <mergeCell ref="O31:W31"/>
     <mergeCell ref="T7:U7"/>
     <mergeCell ref="V7:W7"/>
@@ -8357,14 +8354,18 @@
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="L29:M29"/>
     <mergeCell ref="F30:M30"/>
-    <mergeCell ref="F53:M53"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E48:L48"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="A25:C27"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8410,69 +8411,69 @@
       <c r="E2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="45"/>
+      <c r="M2" s="47"/>
       <c r="O2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="45" t="s">
+      <c r="P2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45" t="s">
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45" t="s">
+      <c r="S2" s="47"/>
+      <c r="T2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45" t="s">
+      <c r="U2" s="47"/>
+      <c r="V2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="45"/>
+      <c r="W2" s="47"/>
     </row>
     <row r="3" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
       <c r="O3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="41" t="s">
+      <c r="P3" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
     </row>
     <row r="4" spans="5:23" ht="30" x14ac:dyDescent="0.25">
       <c r="E4" s="13" t="s">
@@ -9607,11 +9608,11 @@
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
       <c r="E20" s="35" t="s">
         <v>31</v>
       </c>
@@ -9684,9 +9685,9 @@
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
       <c r="E21" s="3"/>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
@@ -9707,10 +9708,10 @@
       <c r="W21" s="28"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="E22" s="43" t="s">
+      <c r="A22" s="45"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="E22" s="48" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="27"/>
@@ -9741,7 +9742,7 @@
       <c r="C23" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="44"/>
+      <c r="E23" s="49"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
@@ -9774,22 +9775,22 @@
       <c r="E24" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F24" s="45" t="s">
+      <c r="F24" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45" t="s">
+      <c r="G24" s="47"/>
+      <c r="H24" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45" t="s">
+      <c r="I24" s="47"/>
+      <c r="J24" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45" t="s">
+      <c r="K24" s="47"/>
+      <c r="L24" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M24" s="45"/>
+      <c r="M24" s="47"/>
       <c r="O24" s="3"/>
       <c r="P24" s="28"/>
       <c r="Q24" s="28"/>
@@ -9814,16 +9815,16 @@
       <c r="E25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="41" t="s">
+      <c r="F25" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
     </row>
     <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -9863,17 +9864,17 @@
       <c r="M26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O26" s="53" t="s">
+      <c r="O26" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="P26" s="54"/>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="54"/>
-      <c r="S26" s="54"/>
-      <c r="T26" s="54"/>
-      <c r="U26" s="54"/>
-      <c r="V26" s="54"/>
-      <c r="W26" s="55"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="52"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -10512,62 +10513,62 @@
       </c>
     </row>
     <row r="43" spans="5:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E43" s="50" t="s">
+      <c r="E43" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="50"/>
-      <c r="L43" s="50"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
       <c r="M43" s="30"/>
       <c r="N43" s="31"/>
     </row>
     <row r="45" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E45" s="43" t="s">
+      <c r="E45" s="48" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E46" s="44"/>
+      <c r="E46" s="49"/>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E47" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F47" s="45" t="s">
+      <c r="F47" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45" t="s">
+      <c r="G47" s="47"/>
+      <c r="H47" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45" t="s">
+      <c r="I47" s="47"/>
+      <c r="J47" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45" t="s">
+      <c r="K47" s="47"/>
+      <c r="L47" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M47" s="45"/>
+      <c r="M47" s="47"/>
     </row>
     <row r="48" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E48" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="41" t="s">
+      <c r="F48" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="42"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
     </row>
     <row r="49" spans="5:13" ht="30" x14ac:dyDescent="0.25">
       <c r="E49" s="13" t="s">
@@ -11187,7 +11188,7 @@
       </c>
     </row>
     <row r="67" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D67" s="49" t="s">
+      <c r="D67" s="41" t="s">
         <v>100</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -11207,7 +11208,7 @@
       </c>
     </row>
     <row r="68" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D68" s="49"/>
+      <c r="D68" s="41"/>
       <c r="E68" s="1" t="s">
         <v>108</v>
       </c>
@@ -11728,11 +11729,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A20:C22"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F48:M48"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E43:L43"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
     <mergeCell ref="O26:W26"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
@@ -11746,14 +11750,11 @@
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="L24:M24"/>
     <mergeCell ref="F25:M25"/>
-    <mergeCell ref="F48:M48"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E43:L43"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="A20:C22"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11799,69 +11800,69 @@
       <c r="E2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="45"/>
+      <c r="M2" s="47"/>
       <c r="O2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="45" t="s">
+      <c r="P2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45" t="s">
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45" t="s">
+      <c r="S2" s="47"/>
+      <c r="T2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45" t="s">
+      <c r="U2" s="47"/>
+      <c r="V2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="45"/>
+      <c r="W2" s="47"/>
     </row>
     <row r="3" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
       <c r="O3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="41" t="s">
+      <c r="P3" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
     </row>
     <row r="4" spans="5:23" ht="30" x14ac:dyDescent="0.25">
       <c r="E4" s="13" t="s">
@@ -12996,11 +12997,11 @@
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
       <c r="E20" s="35" t="s">
         <v>31</v>
       </c>
@@ -13073,9 +13074,9 @@
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
       <c r="E21" s="3"/>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
@@ -13096,10 +13097,10 @@
       <c r="W21" s="28"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="E22" s="43" t="s">
+      <c r="A22" s="45"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="E22" s="48" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="27"/>
@@ -13130,7 +13131,7 @@
       <c r="C23" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="44"/>
+      <c r="E23" s="49"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
@@ -13163,22 +13164,22 @@
       <c r="E24" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F24" s="45" t="s">
+      <c r="F24" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45" t="s">
+      <c r="G24" s="47"/>
+      <c r="H24" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45" t="s">
+      <c r="I24" s="47"/>
+      <c r="J24" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45" t="s">
+      <c r="K24" s="47"/>
+      <c r="L24" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M24" s="45"/>
+      <c r="M24" s="47"/>
       <c r="O24" s="3"/>
       <c r="P24" s="28"/>
       <c r="Q24" s="28"/>
@@ -13203,16 +13204,16 @@
       <c r="E25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="41" t="s">
+      <c r="F25" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
     </row>
     <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -13252,17 +13253,17 @@
       <c r="M26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O26" s="53" t="s">
+      <c r="O26" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="P26" s="54"/>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="54"/>
-      <c r="S26" s="54"/>
-      <c r="T26" s="54"/>
-      <c r="U26" s="54"/>
-      <c r="V26" s="54"/>
-      <c r="W26" s="55"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="52"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -13901,62 +13902,62 @@
       </c>
     </row>
     <row r="43" spans="5:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E43" s="50" t="s">
+      <c r="E43" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="50"/>
-      <c r="L43" s="50"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
       <c r="M43" s="30"/>
       <c r="N43" s="31"/>
     </row>
     <row r="45" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E45" s="43" t="s">
+      <c r="E45" s="48" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E46" s="44"/>
+      <c r="E46" s="49"/>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E47" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F47" s="45" t="s">
+      <c r="F47" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45" t="s">
+      <c r="G47" s="47"/>
+      <c r="H47" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45" t="s">
+      <c r="I47" s="47"/>
+      <c r="J47" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45" t="s">
+      <c r="K47" s="47"/>
+      <c r="L47" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M47" s="45"/>
+      <c r="M47" s="47"/>
     </row>
     <row r="48" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E48" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="41" t="s">
+      <c r="F48" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="42"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
     </row>
     <row r="49" spans="5:13" ht="30" x14ac:dyDescent="0.25">
       <c r="E49" s="13" t="s">
@@ -14576,7 +14577,7 @@
       </c>
     </row>
     <row r="67" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D67" s="49" t="s">
+      <c r="D67" s="41" t="s">
         <v>100</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -14596,7 +14597,7 @@
       </c>
     </row>
     <row r="68" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D68" s="49"/>
+      <c r="D68" s="41"/>
       <c r="E68" s="1" t="s">
         <v>108</v>
       </c>
@@ -15117,11 +15118,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A20:C22"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F48:M48"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E43:L43"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
     <mergeCell ref="O26:W26"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
@@ -15135,14 +15139,11 @@
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="L24:M24"/>
     <mergeCell ref="F25:M25"/>
-    <mergeCell ref="F48:M48"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E43:L43"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="A20:C22"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15188,69 +15189,69 @@
       <c r="E2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="45"/>
+      <c r="M2" s="47"/>
       <c r="O2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="45" t="s">
+      <c r="P2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45" t="s">
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45" t="s">
+      <c r="S2" s="47"/>
+      <c r="T2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45" t="s">
+      <c r="U2" s="47"/>
+      <c r="V2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="45"/>
+      <c r="W2" s="47"/>
     </row>
     <row r="3" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
       <c r="O3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P3" s="41" t="s">
+      <c r="P3" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
     </row>
     <row r="4" spans="5:23" ht="30" x14ac:dyDescent="0.25">
       <c r="E4" s="13" t="s">
@@ -16385,11 +16386,11 @@
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="51" t="s">
+      <c r="A20" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
       <c r="E20" s="35" t="s">
         <v>31</v>
       </c>
@@ -16462,9 +16463,9 @@
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
       <c r="E21" s="3"/>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
@@ -16485,10 +16486,10 @@
       <c r="W21" s="28"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="E22" s="43" t="s">
+      <c r="A22" s="45"/>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="E22" s="48" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="27"/>
@@ -16519,7 +16520,7 @@
       <c r="C23" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="44"/>
+      <c r="E23" s="49"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
@@ -16552,22 +16553,22 @@
       <c r="E24" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F24" s="45" t="s">
+      <c r="F24" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45" t="s">
+      <c r="G24" s="47"/>
+      <c r="H24" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45" t="s">
+      <c r="I24" s="47"/>
+      <c r="J24" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45" t="s">
+      <c r="K24" s="47"/>
+      <c r="L24" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M24" s="45"/>
+      <c r="M24" s="47"/>
       <c r="O24" s="3"/>
       <c r="P24" s="28"/>
       <c r="Q24" s="28"/>
@@ -16592,16 +16593,16 @@
       <c r="E25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="41" t="s">
+      <c r="F25" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
     </row>
     <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -16641,17 +16642,17 @@
       <c r="M26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O26" s="53" t="s">
+      <c r="O26" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="P26" s="54"/>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="54"/>
-      <c r="S26" s="54"/>
-      <c r="T26" s="54"/>
-      <c r="U26" s="54"/>
-      <c r="V26" s="54"/>
-      <c r="W26" s="55"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="52"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -17290,62 +17291,62 @@
       </c>
     </row>
     <row r="43" spans="5:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E43" s="50" t="s">
+      <c r="E43" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="50"/>
-      <c r="L43" s="50"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
       <c r="M43" s="30"/>
       <c r="N43" s="31"/>
     </row>
     <row r="45" spans="5:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E45" s="43" t="s">
+      <c r="E45" s="48" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="46" spans="5:14" x14ac:dyDescent="0.25">
-      <c r="E46" s="44"/>
+      <c r="E46" s="49"/>
     </row>
     <row r="47" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E47" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F47" s="45" t="s">
+      <c r="F47" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45" t="s">
+      <c r="G47" s="47"/>
+      <c r="H47" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45" t="s">
+      <c r="I47" s="47"/>
+      <c r="J47" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45" t="s">
+      <c r="K47" s="47"/>
+      <c r="L47" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M47" s="45"/>
+      <c r="M47" s="47"/>
     </row>
     <row r="48" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E48" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F48" s="41" t="s">
+      <c r="F48" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="42"/>
-      <c r="L48" s="42"/>
-      <c r="M48" s="42"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="43"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
     </row>
     <row r="49" spans="5:13" ht="30" x14ac:dyDescent="0.25">
       <c r="E49" s="13" t="s">
@@ -17965,7 +17966,7 @@
       </c>
     </row>
     <row r="67" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D67" s="49" t="s">
+      <c r="D67" s="41" t="s">
         <v>100</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -17985,7 +17986,7 @@
       </c>
     </row>
     <row r="68" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D68" s="49"/>
+      <c r="D68" s="41"/>
       <c r="E68" s="1" t="s">
         <v>108</v>
       </c>
@@ -18506,11 +18507,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A20:C22"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F48:M48"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E43:L43"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
     <mergeCell ref="O26:W26"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
@@ -18524,14 +18528,11 @@
     <mergeCell ref="J24:K24"/>
     <mergeCell ref="L24:M24"/>
     <mergeCell ref="F25:M25"/>
-    <mergeCell ref="F48:M48"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E43:L43"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="A20:C22"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18545,7 +18546,7 @@
   <dimension ref="D2:W76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18577,69 +18578,69 @@
       <c r="E2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45" t="s">
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45" t="s">
+      <c r="I2" s="47"/>
+      <c r="J2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="45"/>
+      <c r="M2" s="47"/>
       <c r="O2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="45" t="s">
+      <c r="P2" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45" t="s">
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45" t="s">
+      <c r="S2" s="47"/>
+      <c r="T2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45" t="s">
+      <c r="U2" s="47"/>
+      <c r="V2" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="45"/>
+      <c r="W2" s="47"/>
     </row>
     <row r="3" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
       <c r="O3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="P3" s="41" t="s">
+      <c r="P3" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
     </row>
     <row r="4" spans="5:23" ht="30" x14ac:dyDescent="0.25">
       <c r="E4" s="13" t="s">
@@ -19866,7 +19867,7 @@
       <c r="W21" s="28"/>
     </row>
     <row r="23" spans="5:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="43" t="s">
+      <c r="E23" s="48" t="s">
         <v>55</v>
       </c>
       <c r="O23" t="s">
@@ -19877,43 +19878,43 @@
       </c>
     </row>
     <row r="24" spans="5:23" x14ac:dyDescent="0.25">
-      <c r="E24" s="44"/>
+      <c r="E24" s="49"/>
     </row>
     <row r="25" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E25" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F25" s="45" t="s">
+      <c r="F25" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45" t="s">
+      <c r="G25" s="47"/>
+      <c r="H25" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45" t="s">
+      <c r="I25" s="47"/>
+      <c r="J25" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45" t="s">
+      <c r="K25" s="47"/>
+      <c r="L25" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M25" s="45"/>
+      <c r="M25" s="47"/>
     </row>
     <row r="26" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E26" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="41" t="s">
+      <c r="F26" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
     </row>
     <row r="27" spans="5:23" ht="30" x14ac:dyDescent="0.25">
       <c r="E27" s="13" t="s">
@@ -20533,7 +20534,7 @@
       </c>
     </row>
     <row r="45" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D45" s="49" t="s">
+      <c r="D45" s="41" t="s">
         <v>100</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -20553,7 +20554,7 @@
       </c>
     </row>
     <row r="46" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D46" s="49"/>
+      <c r="D46" s="41"/>
       <c r="E46" s="1" t="s">
         <v>63</v>
       </c>
@@ -21082,13 +21083,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F26:M26"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="F3:M3"/>
@@ -21099,6 +21093,2580 @@
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
+    <mergeCell ref="F26:M26"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="D2:W76"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="47"/>
+      <c r="O2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="47"/>
+    </row>
+    <row r="3" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="O3" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="P3" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+    </row>
+    <row r="4" spans="5:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="E4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="20">
+        <f>$F47</f>
+        <v>325573</v>
+      </c>
+      <c r="G5" s="20">
+        <f>$F46</f>
+        <v>467871</v>
+      </c>
+      <c r="H5" s="20">
+        <f>$G47</f>
+        <v>642006</v>
+      </c>
+      <c r="I5" s="20">
+        <f>$G46</f>
+        <v>905224</v>
+      </c>
+      <c r="J5" s="20">
+        <f>$H47</f>
+        <v>19337433</v>
+      </c>
+      <c r="K5" s="20">
+        <f>$H46</f>
+        <v>27688889</v>
+      </c>
+      <c r="L5" s="20">
+        <f>$I47</f>
+        <v>19813662908</v>
+      </c>
+      <c r="M5" s="20">
+        <f>$I46</f>
+        <v>28347256279</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="22">
+        <f>F5*($P$23)/4096</f>
+        <v>214.61110839843752</v>
+      </c>
+      <c r="Q5" s="22">
+        <f>G5*($P$23)/4096</f>
+        <v>308.41105957031255</v>
+      </c>
+      <c r="R5" s="22">
+        <f>H5*($P$23)/32768</f>
+        <v>52.899664306640631</v>
+      </c>
+      <c r="S5" s="22">
+        <f>I5*($P$23)/32768</f>
+        <v>74.588159179687509</v>
+      </c>
+      <c r="T5" s="22">
+        <f>J5*($P$23)/(1048576)</f>
+        <v>49.792355632781984</v>
+      </c>
+      <c r="U5" s="22">
+        <f>K5*($P$23)/(1048576)</f>
+        <v>71.296692180633556</v>
+      </c>
+      <c r="V5" s="22">
+        <f>L5*($P$23)/1073741824</f>
+        <v>49.822861190512782</v>
+      </c>
+      <c r="W5" s="22">
+        <f>M5*($P$23)/1073741824</f>
+        <v>71.28118719281629</v>
+      </c>
+    </row>
+    <row r="6" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E6" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="19">
+        <f>$F49</f>
+        <v>245872</v>
+      </c>
+      <c r="G6" s="19">
+        <f>$F48</f>
+        <v>416389</v>
+      </c>
+      <c r="H6" s="19">
+        <f>$G49</f>
+        <v>467775</v>
+      </c>
+      <c r="I6" s="19">
+        <f>$G48</f>
+        <v>762633</v>
+      </c>
+      <c r="J6" s="19">
+        <f>$H49</f>
+        <v>13262745</v>
+      </c>
+      <c r="K6" s="19">
+        <f>$H48</f>
+        <v>23151129</v>
+      </c>
+      <c r="L6" s="19">
+        <f>$I49</f>
+        <v>13519289191</v>
+      </c>
+      <c r="M6" s="19">
+        <f>$I48</f>
+        <v>24236669408</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="22">
+        <f t="shared" ref="P6:Q20" si="0">F6*($P$23)/4096</f>
+        <v>162.07382812500001</v>
+      </c>
+      <c r="Q6" s="22">
+        <f t="shared" si="0"/>
+        <v>274.47517089843751</v>
+      </c>
+      <c r="R6" s="22">
+        <f t="shared" ref="R6:S20" si="1">H6*($P$23)/32768</f>
+        <v>38.543472290039062</v>
+      </c>
+      <c r="S6" s="22">
+        <f t="shared" si="1"/>
+        <v>62.83902282714844</v>
+      </c>
+      <c r="T6" s="22">
+        <f t="shared" ref="T6:U20" si="2">J6*($P$23)/(1048576)</f>
+        <v>34.150516033172607</v>
+      </c>
+      <c r="U6" s="22">
+        <f t="shared" si="2"/>
+        <v>59.612320232391362</v>
+      </c>
+      <c r="V6" s="22">
+        <f t="shared" ref="V6:W20" si="3">L6*($P$23)/1073741824</f>
+        <v>33.995211884099994</v>
+      </c>
+      <c r="W6" s="22">
+        <f t="shared" si="3"/>
+        <v>60.944824853539473</v>
+      </c>
+    </row>
+    <row r="7" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E7" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="19">
+        <f>$F50</f>
+        <v>45946</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="19">
+        <f>$G50</f>
+        <v>345899</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="19">
+        <f>$H50</f>
+        <v>11067563</v>
+      </c>
+      <c r="K7" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="19">
+        <f>$I50</f>
+        <v>11415155203</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="P7" s="22">
+        <f t="shared" si="0"/>
+        <v>30.286669921875003</v>
+      </c>
+      <c r="Q7" s="22" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R7" s="22">
+        <f t="shared" si="1"/>
+        <v>28.501199340820314</v>
+      </c>
+      <c r="S7" s="22" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T7" s="22">
+        <f t="shared" si="2"/>
+        <v>28.498096561431886</v>
+      </c>
+      <c r="U7" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V7" s="22">
+        <f t="shared" si="3"/>
+        <v>28.704217679891737</v>
+      </c>
+      <c r="W7" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E8" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="21">
+        <f>$F52</f>
+        <v>4612488</v>
+      </c>
+      <c r="G8" s="19">
+        <f>$F51</f>
+        <v>724337</v>
+      </c>
+      <c r="H8" s="21">
+        <f>$G52</f>
+        <v>10222808</v>
+      </c>
+      <c r="I8" s="19">
+        <f>$G51</f>
+        <v>1250016</v>
+      </c>
+      <c r="J8" s="21">
+        <f>$H52</f>
+        <v>319591894</v>
+      </c>
+      <c r="K8" s="19">
+        <f>$H51</f>
+        <v>38635284</v>
+      </c>
+      <c r="L8" s="21">
+        <f>$I52</f>
+        <v>328405658363</v>
+      </c>
+      <c r="M8" s="19">
+        <f>$I51</f>
+        <v>39538634572</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" s="22">
+        <f t="shared" si="0"/>
+        <v>3040.4583984375004</v>
+      </c>
+      <c r="Q8" s="22">
+        <f t="shared" si="0"/>
+        <v>477.46823730468753</v>
+      </c>
+      <c r="R8" s="22">
+        <f t="shared" si="1"/>
+        <v>842.33342285156255</v>
+      </c>
+      <c r="S8" s="22">
+        <f t="shared" si="1"/>
+        <v>102.99814453125001</v>
+      </c>
+      <c r="T8" s="22">
+        <f t="shared" si="2"/>
+        <v>822.92376880645759</v>
+      </c>
+      <c r="U8" s="22">
+        <f t="shared" si="2"/>
+        <v>99.482790756225597</v>
+      </c>
+      <c r="V8" s="22">
+        <f t="shared" si="3"/>
+        <v>825.79932881528521</v>
+      </c>
+      <c r="W8" s="22">
+        <f t="shared" si="3"/>
+        <v>99.422701955214151</v>
+      </c>
+    </row>
+    <row r="9" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E9" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="21">
+        <f>$F54</f>
+        <v>73141</v>
+      </c>
+      <c r="G9" s="19">
+        <f>$F53</f>
+        <v>114374</v>
+      </c>
+      <c r="H9" s="21">
+        <f>$G54</f>
+        <v>159404</v>
+      </c>
+      <c r="I9" s="19">
+        <f>$G53</f>
+        <v>214091</v>
+      </c>
+      <c r="J9" s="21">
+        <f>$H54</f>
+        <v>5199406</v>
+      </c>
+      <c r="K9" s="19">
+        <f>$H53</f>
+        <v>6895937</v>
+      </c>
+      <c r="L9" s="21">
+        <f>$I54</f>
+        <v>5193637037</v>
+      </c>
+      <c r="M9" s="19">
+        <f>$I53</f>
+        <v>7069066112</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="22">
+        <f t="shared" si="0"/>
+        <v>48.213061523437503</v>
+      </c>
+      <c r="Q9" s="22">
+        <f t="shared" si="0"/>
+        <v>75.393017578125011</v>
+      </c>
+      <c r="R9" s="22">
+        <f t="shared" si="1"/>
+        <v>13.134484863281251</v>
+      </c>
+      <c r="S9" s="22">
+        <f t="shared" si="1"/>
+        <v>17.640554809570315</v>
+      </c>
+      <c r="T9" s="22">
+        <f t="shared" si="2"/>
+        <v>13.388057899475099</v>
+      </c>
+      <c r="U9" s="22">
+        <f t="shared" si="2"/>
+        <v>17.756490612030031</v>
+      </c>
+      <c r="V9" s="22">
+        <f t="shared" si="3"/>
+        <v>13.059768825676294</v>
+      </c>
+      <c r="W9" s="22">
+        <f t="shared" si="3"/>
+        <v>17.775668299198152</v>
+      </c>
+    </row>
+    <row r="10" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E10" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="21">
+        <f>$F56</f>
+        <v>47428</v>
+      </c>
+      <c r="G10" s="19">
+        <f>$F55</f>
+        <v>53547</v>
+      </c>
+      <c r="H10" s="21">
+        <f>$G56</f>
+        <v>88113</v>
+      </c>
+      <c r="I10" s="19">
+        <f>$G55</f>
+        <v>99120</v>
+      </c>
+      <c r="J10" s="21">
+        <f>$H56</f>
+        <v>2837823</v>
+      </c>
+      <c r="K10" s="19">
+        <f>$H55</f>
+        <v>3064694</v>
+      </c>
+      <c r="L10" s="21">
+        <f>$I56</f>
+        <v>2906605823</v>
+      </c>
+      <c r="M10" s="19">
+        <f>$I55</f>
+        <v>3160653145</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="22">
+        <f t="shared" si="0"/>
+        <v>31.263574218750001</v>
+      </c>
+      <c r="Q10" s="22">
+        <f t="shared" si="0"/>
+        <v>35.297094726562506</v>
+      </c>
+      <c r="R10" s="22">
+        <f t="shared" si="1"/>
+        <v>7.2602874755859377</v>
+      </c>
+      <c r="S10" s="22">
+        <f t="shared" si="1"/>
+        <v>8.167236328125</v>
+      </c>
+      <c r="T10" s="22">
+        <f t="shared" si="2"/>
+        <v>7.3071690559387212</v>
+      </c>
+      <c r="U10" s="22">
+        <f t="shared" si="2"/>
+        <v>7.8913438796997077</v>
+      </c>
+      <c r="V10" s="22">
+        <f t="shared" si="3"/>
+        <v>7.3088665698654953</v>
+      </c>
+      <c r="W10" s="22">
+        <f t="shared" si="3"/>
+        <v>7.9476865860633561</v>
+      </c>
+    </row>
+    <row r="11" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E11" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="21">
+        <f>$F58</f>
+        <v>185079</v>
+      </c>
+      <c r="G11" s="19">
+        <f>$F57</f>
+        <v>295810</v>
+      </c>
+      <c r="H11" s="21">
+        <f>$G58</f>
+        <v>330195</v>
+      </c>
+      <c r="I11" s="19">
+        <f>$G57</f>
+        <v>421117</v>
+      </c>
+      <c r="J11" s="21">
+        <f>$H58</f>
+        <v>10486435</v>
+      </c>
+      <c r="K11" s="19">
+        <f>$H57</f>
+        <v>11302145</v>
+      </c>
+      <c r="L11" s="21">
+        <f>$I58</f>
+        <v>10759583722</v>
+      </c>
+      <c r="M11" s="19">
+        <f>$I57</f>
+        <v>11610571201</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="22">
+        <f t="shared" si="0"/>
+        <v>122.00031738281251</v>
+      </c>
+      <c r="Q11" s="22">
+        <f t="shared" si="0"/>
+        <v>194.991943359375</v>
+      </c>
+      <c r="R11" s="22">
+        <f t="shared" si="1"/>
+        <v>27.207229614257816</v>
+      </c>
+      <c r="S11" s="22">
+        <f t="shared" si="1"/>
+        <v>34.698971557617192</v>
+      </c>
+      <c r="T11" s="22">
+        <f t="shared" si="2"/>
+        <v>27.00173807144165</v>
+      </c>
+      <c r="U11" s="22">
+        <f t="shared" si="2"/>
+        <v>29.102126598358158</v>
+      </c>
+      <c r="V11" s="22">
+        <f t="shared" si="3"/>
+        <v>27.055736677162351</v>
+      </c>
+      <c r="W11" s="22">
+        <f t="shared" si="3"/>
+        <v>29.195605071913452</v>
+      </c>
+    </row>
+    <row r="12" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E12" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="21">
+        <f>$F60</f>
+        <v>187530</v>
+      </c>
+      <c r="G12" s="19">
+        <f>$F59</f>
+        <v>246864</v>
+      </c>
+      <c r="H12" s="21">
+        <f>$G60</f>
+        <v>327735</v>
+      </c>
+      <c r="I12" s="19">
+        <f>$G59</f>
+        <v>297003</v>
+      </c>
+      <c r="J12" s="21">
+        <f>$H60</f>
+        <v>10389359</v>
+      </c>
+      <c r="K12" s="19">
+        <f>$H59</f>
+        <v>9149518</v>
+      </c>
+      <c r="L12" s="21">
+        <f>$I60</f>
+        <v>10662335639</v>
+      </c>
+      <c r="M12" s="19">
+        <f>$I59</f>
+        <v>9395542413</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" s="22">
+        <f t="shared" si="0"/>
+        <v>123.61596679687501</v>
+      </c>
+      <c r="Q12" s="22">
+        <f t="shared" si="0"/>
+        <v>162.72773437500001</v>
+      </c>
+      <c r="R12" s="22">
+        <f t="shared" si="1"/>
+        <v>27.004531860351562</v>
+      </c>
+      <c r="S12" s="22">
+        <f t="shared" si="1"/>
+        <v>24.472293090820315</v>
+      </c>
+      <c r="T12" s="22">
+        <f t="shared" si="2"/>
+        <v>26.751775074005128</v>
+      </c>
+      <c r="U12" s="22">
+        <f t="shared" si="2"/>
+        <v>23.559282875061037</v>
+      </c>
+      <c r="V12" s="22">
+        <f t="shared" si="3"/>
+        <v>26.811199472565207</v>
+      </c>
+      <c r="W12" s="22">
+        <f t="shared" si="3"/>
+        <v>23.625758024957033</v>
+      </c>
+    </row>
+    <row r="13" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E13" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="21">
+        <f>$F62</f>
+        <v>336187</v>
+      </c>
+      <c r="G13" s="19">
+        <f>$F61</f>
+        <v>724918</v>
+      </c>
+      <c r="H13" s="21">
+        <f>$G62</f>
+        <v>648834</v>
+      </c>
+      <c r="I13" s="19">
+        <f>$G61</f>
+        <v>1373025</v>
+      </c>
+      <c r="J13" s="21">
+        <f>$H62</f>
+        <v>20034640</v>
+      </c>
+      <c r="K13" s="19">
+        <f>$H61</f>
+        <v>42980837</v>
+      </c>
+      <c r="L13" s="21">
+        <f>$I62</f>
+        <v>20572719936</v>
+      </c>
+      <c r="M13" s="19">
+        <f>$I61</f>
+        <v>43711831102</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P13" s="22">
+        <f t="shared" si="0"/>
+        <v>221.60764160156251</v>
+      </c>
+      <c r="Q13" s="22">
+        <f t="shared" si="0"/>
+        <v>477.85122070312502</v>
+      </c>
+      <c r="R13" s="22">
+        <f t="shared" si="1"/>
+        <v>53.462274169921876</v>
+      </c>
+      <c r="S13" s="22">
+        <f t="shared" si="1"/>
+        <v>113.13377380371095</v>
+      </c>
+      <c r="T13" s="22">
+        <f t="shared" si="2"/>
+        <v>51.587608337402344</v>
+      </c>
+      <c r="U13" s="22">
+        <f t="shared" si="2"/>
+        <v>110.67224493026734</v>
+      </c>
+      <c r="V13" s="22">
+        <f t="shared" si="3"/>
+        <v>51.731563943624501</v>
+      </c>
+      <c r="W13" s="22">
+        <f t="shared" si="3"/>
+        <v>109.9165007242933</v>
+      </c>
+    </row>
+    <row r="14" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E14" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="21">
+        <f>$F64</f>
+        <v>255644</v>
+      </c>
+      <c r="G14" s="19">
+        <f>$F63</f>
+        <v>324376</v>
+      </c>
+      <c r="H14" s="21">
+        <f>$G64</f>
+        <v>478206</v>
+      </c>
+      <c r="I14" s="19">
+        <f>$G63</f>
+        <v>608575</v>
+      </c>
+      <c r="J14" s="21">
+        <f>$H64</f>
+        <v>15386647</v>
+      </c>
+      <c r="K14" s="19">
+        <f>$H63</f>
+        <v>19670244</v>
+      </c>
+      <c r="L14" s="21">
+        <f>$I64</f>
+        <v>15737515881</v>
+      </c>
+      <c r="M14" s="19">
+        <f>$I63</f>
+        <v>20201018591</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="22">
+        <f t="shared" si="0"/>
+        <v>168.51533203125001</v>
+      </c>
+      <c r="Q14" s="22">
+        <f t="shared" si="0"/>
+        <v>213.82207031250002</v>
+      </c>
+      <c r="R14" s="22">
+        <f t="shared" si="1"/>
+        <v>39.402960205078131</v>
+      </c>
+      <c r="S14" s="22">
+        <f t="shared" si="1"/>
+        <v>50.145034790039063</v>
+      </c>
+      <c r="T14" s="22">
+        <f t="shared" si="2"/>
+        <v>39.619395160675055</v>
+      </c>
+      <c r="U14" s="22">
+        <f t="shared" si="2"/>
+        <v>50.649317550659184</v>
+      </c>
+      <c r="V14" s="22">
+        <f t="shared" si="3"/>
+        <v>39.573100282531236</v>
+      </c>
+      <c r="W14" s="22">
+        <f t="shared" si="3"/>
+        <v>50.796894538868223</v>
+      </c>
+    </row>
+    <row r="15" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E15" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="21">
+        <f>$F66</f>
+        <v>239864</v>
+      </c>
+      <c r="G15" s="19">
+        <f>$F65</f>
+        <v>539166</v>
+      </c>
+      <c r="H15" s="21">
+        <f>$G66</f>
+        <v>448755</v>
+      </c>
+      <c r="I15" s="19">
+        <f>$G65</f>
+        <v>1023616</v>
+      </c>
+      <c r="J15" s="21">
+        <f>$H66</f>
+        <v>14442141</v>
+      </c>
+      <c r="K15" s="19">
+        <f>$H65</f>
+        <v>31696181</v>
+      </c>
+      <c r="L15" s="21">
+        <f>$I66</f>
+        <v>14832493094</v>
+      </c>
+      <c r="M15" s="19">
+        <f>$I65</f>
+        <v>32533269848</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P15" s="22">
+        <f t="shared" si="0"/>
+        <v>158.11347656250001</v>
+      </c>
+      <c r="Q15" s="22">
+        <f t="shared" si="0"/>
+        <v>355.40727539062505</v>
+      </c>
+      <c r="R15" s="22">
+        <f t="shared" si="1"/>
+        <v>36.976272583007813</v>
+      </c>
+      <c r="S15" s="22">
+        <f t="shared" si="1"/>
+        <v>84.343359375000006</v>
+      </c>
+      <c r="T15" s="22">
+        <f t="shared" si="2"/>
+        <v>37.187367153167727</v>
+      </c>
+      <c r="U15" s="22">
+        <f t="shared" si="2"/>
+        <v>81.615151119232181</v>
+      </c>
+      <c r="V15" s="22">
+        <f t="shared" si="3"/>
+        <v>37.297356271930042</v>
+      </c>
+      <c r="W15" s="22">
+        <f t="shared" si="3"/>
+        <v>81.807215315848595</v>
+      </c>
+    </row>
+    <row r="16" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E16" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="21">
+        <f>$F68</f>
+        <v>1443903</v>
+      </c>
+      <c r="G16" s="19">
+        <f>$F67</f>
+        <v>1179086</v>
+      </c>
+      <c r="H16" s="21">
+        <f>$G68</f>
+        <v>2625745</v>
+      </c>
+      <c r="I16" s="19">
+        <f>$G67</f>
+        <v>1850759</v>
+      </c>
+      <c r="J16" s="21">
+        <f>$H68</f>
+        <v>85117718</v>
+      </c>
+      <c r="K16" s="19">
+        <f>$H67</f>
+        <v>63590353</v>
+      </c>
+      <c r="L16" s="21">
+        <f>$I68</f>
+        <v>86518744395</v>
+      </c>
+      <c r="M16" s="19">
+        <f>$I67</f>
+        <v>65162667832</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P16" s="22">
+        <f t="shared" si="0"/>
+        <v>951.79152832031252</v>
+      </c>
+      <c r="Q16" s="22">
+        <f t="shared" si="0"/>
+        <v>777.22954101562505</v>
+      </c>
+      <c r="R16" s="22">
+        <f t="shared" si="1"/>
+        <v>216.35472106933597</v>
+      </c>
+      <c r="S16" s="22">
+        <f t="shared" si="1"/>
+        <v>152.49784240722659</v>
+      </c>
+      <c r="T16" s="22">
+        <f t="shared" si="2"/>
+        <v>219.17137012481692</v>
+      </c>
+      <c r="U16" s="22">
+        <f t="shared" si="2"/>
+        <v>163.74011335372927</v>
+      </c>
+      <c r="V16" s="22">
+        <f t="shared" si="3"/>
+        <v>217.55752141261476</v>
+      </c>
+      <c r="W16" s="22">
+        <f t="shared" si="3"/>
+        <v>163.85615165010097</v>
+      </c>
+    </row>
+    <row r="17" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E17" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="21">
+        <f>$F70</f>
+        <v>18271</v>
+      </c>
+      <c r="G17" s="19">
+        <f>$F69</f>
+        <v>28404</v>
+      </c>
+      <c r="H17" s="21">
+        <f>$G70</f>
+        <v>145772</v>
+      </c>
+      <c r="I17" s="19">
+        <f>$G69</f>
+        <v>213424</v>
+      </c>
+      <c r="J17" s="21">
+        <f>$H70</f>
+        <v>4418369</v>
+      </c>
+      <c r="K17" s="19">
+        <f>$H69</f>
+        <v>6848843</v>
+      </c>
+      <c r="L17" s="21">
+        <f>$I70</f>
+        <v>4837830877</v>
+      </c>
+      <c r="M17" s="19">
+        <f>$I69</f>
+        <v>7024500305</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P17" s="22">
+        <f t="shared" si="0"/>
+        <v>12.043872070312501</v>
+      </c>
+      <c r="Q17" s="22">
+        <f t="shared" si="0"/>
+        <v>18.723339843750001</v>
+      </c>
+      <c r="R17" s="22">
+        <f t="shared" si="1"/>
+        <v>12.011242675781251</v>
+      </c>
+      <c r="S17" s="22">
+        <f t="shared" si="1"/>
+        <v>17.585595703125001</v>
+      </c>
+      <c r="T17" s="22">
+        <f t="shared" si="2"/>
+        <v>11.37694959640503</v>
+      </c>
+      <c r="U17" s="22">
+        <f t="shared" si="2"/>
+        <v>17.635227298736574</v>
+      </c>
+      <c r="V17" s="22">
+        <f t="shared" si="3"/>
+        <v>12.165068991389127</v>
+      </c>
+      <c r="W17" s="22">
+        <f t="shared" si="3"/>
+        <v>17.663604415487498</v>
+      </c>
+    </row>
+    <row r="18" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E18" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="21">
+        <f>$F72</f>
+        <v>40065</v>
+      </c>
+      <c r="G18" s="19">
+        <f>$F71</f>
+        <v>58089</v>
+      </c>
+      <c r="H18" s="21">
+        <f>$G72</f>
+        <v>300929</v>
+      </c>
+      <c r="I18" s="19">
+        <f>$G71</f>
+        <v>431361</v>
+      </c>
+      <c r="J18" s="21">
+        <f>$H72</f>
+        <v>9682761</v>
+      </c>
+      <c r="K18" s="19">
+        <f>$H71</f>
+        <v>13890734</v>
+      </c>
+      <c r="L18" s="21">
+        <f>$I72</f>
+        <v>9934200695</v>
+      </c>
+      <c r="M18" s="19">
+        <f>$I71</f>
+        <v>14228312927</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P18" s="22">
+        <f t="shared" si="0"/>
+        <v>26.4100341796875</v>
+      </c>
+      <c r="Q18" s="22">
+        <f t="shared" si="0"/>
+        <v>38.291088867187504</v>
+      </c>
+      <c r="R18" s="22">
+        <f t="shared" si="1"/>
+        <v>24.795785522460939</v>
+      </c>
+      <c r="S18" s="22">
+        <f t="shared" si="1"/>
+        <v>35.543051147460943</v>
+      </c>
+      <c r="T18" s="22">
+        <f t="shared" si="2"/>
+        <v>24.932341289520267</v>
+      </c>
+      <c r="U18" s="22">
+        <f t="shared" si="2"/>
+        <v>35.767537879943852</v>
+      </c>
+      <c r="V18" s="22">
+        <f t="shared" si="3"/>
+        <v>24.980252493638545</v>
+      </c>
+      <c r="W18" s="22">
+        <f t="shared" si="3"/>
+        <v>35.778102374542506</v>
+      </c>
+    </row>
+    <row r="19" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E19" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="21">
+        <f>$F74</f>
+        <v>1074250</v>
+      </c>
+      <c r="G19" s="19">
+        <f>$F73</f>
+        <v>172111</v>
+      </c>
+      <c r="H19" s="21">
+        <f>$G74</f>
+        <v>9987447</v>
+      </c>
+      <c r="I19" s="19">
+        <f>$G73</f>
+        <v>1228716</v>
+      </c>
+      <c r="J19" s="21">
+        <f>$H74</f>
+        <v>322383123</v>
+      </c>
+      <c r="K19" s="19">
+        <f>$H73</f>
+        <v>41247225</v>
+      </c>
+      <c r="L19" s="21">
+        <f>$I74</f>
+        <v>325961523696</v>
+      </c>
+      <c r="M19" s="19">
+        <f>$I73</f>
+        <v>40396150764</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P19" s="22">
+        <f t="shared" si="0"/>
+        <v>708.123779296875</v>
+      </c>
+      <c r="Q19" s="22">
+        <f t="shared" si="0"/>
+        <v>113.4520751953125</v>
+      </c>
+      <c r="R19" s="22">
+        <f t="shared" si="1"/>
+        <v>822.94027404785163</v>
+      </c>
+      <c r="S19" s="22">
+        <f t="shared" si="1"/>
+        <v>101.24307861328126</v>
+      </c>
+      <c r="T19" s="22">
+        <f t="shared" si="2"/>
+        <v>830.11096200942995</v>
+      </c>
+      <c r="U19" s="22">
+        <f t="shared" si="2"/>
+        <v>106.20833158493042</v>
+      </c>
+      <c r="V19" s="22">
+        <f t="shared" si="3"/>
+        <v>819.65337878018624</v>
+      </c>
+      <c r="W19" s="22">
+        <f t="shared" si="3"/>
+        <v>101.57898726202548</v>
+      </c>
+    </row>
+    <row r="20" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E20" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="21">
+        <f>$F76</f>
+        <v>19537</v>
+      </c>
+      <c r="G20" s="19">
+        <f>$F75</f>
+        <v>27335</v>
+      </c>
+      <c r="H20" s="21">
+        <f>$G76</f>
+        <v>139828</v>
+      </c>
+      <c r="I20" s="19">
+        <f>$G75</f>
+        <v>203828</v>
+      </c>
+      <c r="J20" s="21">
+        <f>$H76</f>
+        <v>4540382</v>
+      </c>
+      <c r="K20" s="19">
+        <f>$H75</f>
+        <v>6568998</v>
+      </c>
+      <c r="L20" s="21">
+        <f>$I76</f>
+        <v>4574343064</v>
+      </c>
+      <c r="M20" s="19">
+        <f>$I75</f>
+        <v>6718536265</v>
+      </c>
+      <c r="O20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="P20" s="22">
+        <f t="shared" si="0"/>
+        <v>12.8783935546875</v>
+      </c>
+      <c r="Q20" s="22">
+        <f t="shared" si="0"/>
+        <v>18.0186767578125</v>
+      </c>
+      <c r="R20" s="22">
+        <f t="shared" si="1"/>
+        <v>11.521472167968751</v>
+      </c>
+      <c r="S20" s="22">
+        <f t="shared" si="1"/>
+        <v>16.794909667968753</v>
+      </c>
+      <c r="T20" s="22">
+        <f t="shared" si="2"/>
+        <v>11.691123390197754</v>
+      </c>
+      <c r="U20" s="22">
+        <f t="shared" si="2"/>
+        <v>16.914648628234865</v>
+      </c>
+      <c r="V20" s="22">
+        <f t="shared" si="3"/>
+        <v>11.50251019075513</v>
+      </c>
+      <c r="W20" s="22">
+        <f t="shared" si="3"/>
+        <v>16.894236128311604</v>
+      </c>
+    </row>
+    <row r="21" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="27"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="28"/>
+    </row>
+    <row r="23" spans="5:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="O23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P23">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="24" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E24" s="49"/>
+    </row>
+    <row r="25" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E25" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="M25" s="47"/>
+    </row>
+    <row r="26" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E26" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+    </row>
+    <row r="27" spans="5:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="E27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E28" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="20">
+        <f>(((4*1024*4)/(1024*1024))/F5)*10^9</f>
+        <v>47.992308944537783</v>
+      </c>
+      <c r="G28" s="20">
+        <f>(((4096*8)/(1024*1024))/G5)*10^9</f>
+        <v>66.791914865422314</v>
+      </c>
+      <c r="H28" s="20">
+        <f>(((32*1024*4)/(1024*1024))/H5)*10^9</f>
+        <v>194.70223019722556</v>
+      </c>
+      <c r="I28" s="20">
+        <f>(((32*1024*8)/(1024*1024))/I5)*10^9</f>
+        <v>276.17473686071071</v>
+      </c>
+      <c r="J28" s="20">
+        <f>(((1*1024*1024*8)/(1024*1024))/J5)*10^9</f>
+        <v>413.70537650990178</v>
+      </c>
+      <c r="K28" s="20">
+        <f>(((1*1024*1024*8)/(1024*1024))/K5)*10^9</f>
+        <v>288.92455742807158</v>
+      </c>
+      <c r="L28" s="20">
+        <f>(((1*1024*1024*1024*4)/(1024*1024))/L5)*10^9</f>
+        <v>206.72603642339104</v>
+      </c>
+      <c r="M28" s="20">
+        <f>(((1*1024*1024*1024*8)/(1024*1024))/M5)*10^9</f>
+        <v>288.98740390860104</v>
+      </c>
+    </row>
+    <row r="29" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E29" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="20">
+        <f>(((4*1024*4)/(1024*1024))/F6)*10^9</f>
+        <v>63.549326478818251</v>
+      </c>
+      <c r="G29" s="20">
+        <f>(((4096*8)/(1024*1024))/G6)*10^9</f>
+        <v>75.050013328882358</v>
+      </c>
+      <c r="H29" s="20">
+        <f>(((32*1024*4)/(1024*1024))/H6)*10^9</f>
+        <v>267.2224894447117</v>
+      </c>
+      <c r="I29" s="20">
+        <f>(((32*1024*8)/(1024*1024))/I6)*10^9</f>
+        <v>327.8116735048182</v>
+      </c>
+      <c r="J29" s="20">
+        <f>(((1*1024*1024*4)/(1024*1024))/J6)*10^9</f>
+        <v>301.5966905795143</v>
+      </c>
+      <c r="K29" s="20">
+        <f>(((1*1024*1024*8)/(1024*1024))/K6)*10^9</f>
+        <v>345.55550185047133</v>
+      </c>
+      <c r="L29" s="20">
+        <f>(((1*1024*1024*1024*4)/(1024*1024))/L6)*10^9</f>
+        <v>302.97450865440254</v>
+      </c>
+      <c r="M29" s="20">
+        <f>(((1*1024*1024*1024*8)/(1024*1024))/M6)*10^9</f>
+        <v>338.00023683518157</v>
+      </c>
+    </row>
+    <row r="30" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E30" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="20">
+        <f>(((4*1024)/(1024*1024))/F7)*10^9</f>
+        <v>85.018282331432545</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H30" s="20">
+        <f>(((32*1024)/(1024*1024))/H7)*10^9</f>
+        <v>90.344291252648901</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J30" s="20">
+        <f>(((1*1024*1024)/(1024*1024))/J7)*10^9</f>
+        <v>90.354127643095424</v>
+      </c>
+      <c r="K30" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="L30" s="20">
+        <f>(((1*1024*1024*1024)/(1024*1024))/L7)*10^9</f>
+        <v>89.705306830246528</v>
+      </c>
+      <c r="M30" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="20">
+        <f t="shared" ref="F31:F43" si="4">(((4*1024*4)/(1024*1024))/F8)*10^9</f>
+        <v>3.3875426884579429</v>
+      </c>
+      <c r="G31" s="20">
+        <f t="shared" ref="G31:G43" si="5">(((4096*8)/(1024*1024))/G8)*10^9</f>
+        <v>43.142901715637883</v>
+      </c>
+      <c r="H31" s="20">
+        <f t="shared" ref="H31:H43" si="6">(((32*1024*4)/(1024*1024))/H8)*10^9</f>
+        <v>12.227560177203758</v>
+      </c>
+      <c r="I31" s="20">
+        <f t="shared" ref="I31:I43" si="7">(((32*1024*8)/(1024*1024))/I8)*10^9</f>
+        <v>199.99744003276757</v>
+      </c>
+      <c r="J31" s="20">
+        <f t="shared" ref="J31:J43" si="8">(((1*1024*1024*4)/(1024*1024))/J8)*10^9</f>
+        <v>12.515961997459172</v>
+      </c>
+      <c r="K31" s="20">
+        <f t="shared" ref="K31:K43" si="9">(((1*1024*1024*8)/(1024*1024))/K8)*10^9</f>
+        <v>207.06460964542151</v>
+      </c>
+      <c r="L31" s="20">
+        <f t="shared" ref="L31:L43" si="10">(((1*1024*1024*1024*4)/(1024*1024))/L8)*10^9</f>
+        <v>12.472379496800651</v>
+      </c>
+      <c r="M31" s="20">
+        <f t="shared" ref="M31:M43" si="11">(((1*1024*1024*1024*8)/(1024*1024))/M8)*10^9</f>
+        <v>207.18975474690046</v>
+      </c>
+    </row>
+    <row r="32" spans="5:23" x14ac:dyDescent="0.25">
+      <c r="E32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="20">
+        <f t="shared" si="4"/>
+        <v>213.62847103539738</v>
+      </c>
+      <c r="G32" s="20">
+        <f t="shared" si="5"/>
+        <v>273.22643258083127</v>
+      </c>
+      <c r="H32" s="20">
+        <f t="shared" si="6"/>
+        <v>784.17103711324683</v>
+      </c>
+      <c r="I32" s="20">
+        <f t="shared" si="7"/>
+        <v>1167.7277419415109</v>
+      </c>
+      <c r="J32" s="20">
+        <f t="shared" si="8"/>
+        <v>769.31864909183855</v>
+      </c>
+      <c r="K32" s="20">
+        <f t="shared" si="9"/>
+        <v>1160.1034058170776</v>
+      </c>
+      <c r="L32" s="20">
+        <f t="shared" si="10"/>
+        <v>788.65734567504012</v>
+      </c>
+      <c r="M32" s="20">
+        <f t="shared" si="11"/>
+        <v>1158.8518016678015</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="20">
+        <f t="shared" si="4"/>
+        <v>329.44674032217256</v>
+      </c>
+      <c r="G33" s="20">
+        <f t="shared" si="5"/>
+        <v>583.59945468466958</v>
+      </c>
+      <c r="H33" s="20">
+        <f t="shared" si="6"/>
+        <v>1418.6328918547774</v>
+      </c>
+      <c r="I33" s="20">
+        <f t="shared" si="7"/>
+        <v>2522.1953188054886</v>
+      </c>
+      <c r="J33" s="20">
+        <f t="shared" si="8"/>
+        <v>1409.5311793582616</v>
+      </c>
+      <c r="K33" s="20">
+        <f t="shared" si="9"/>
+        <v>2610.3748041403155</v>
+      </c>
+      <c r="L33" s="20">
+        <f t="shared" si="10"/>
+        <v>1409.2038100207164</v>
+      </c>
+      <c r="M33" s="20">
+        <f t="shared" si="11"/>
+        <v>2591.8693460430309</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E34" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" s="20">
+        <f t="shared" si="4"/>
+        <v>84.423408382366446</v>
+      </c>
+      <c r="G34" s="20">
+        <f t="shared" si="5"/>
+        <v>105.64213515432203</v>
+      </c>
+      <c r="H34" s="20">
+        <f t="shared" si="6"/>
+        <v>378.56418177137749</v>
+      </c>
+      <c r="I34" s="20">
+        <f t="shared" si="7"/>
+        <v>593.65924434302099</v>
+      </c>
+      <c r="J34" s="20">
+        <f t="shared" si="8"/>
+        <v>381.44517178621714</v>
+      </c>
+      <c r="K34" s="20">
+        <f t="shared" si="9"/>
+        <v>707.83023930413208</v>
+      </c>
+      <c r="L34" s="20">
+        <f t="shared" si="10"/>
+        <v>380.68387270642774</v>
+      </c>
+      <c r="M34" s="20">
+        <f t="shared" si="11"/>
+        <v>705.56390880187155</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="20">
+        <f t="shared" si="4"/>
+        <v>83.320002132992045</v>
+      </c>
+      <c r="G35" s="20">
+        <f t="shared" si="5"/>
+        <v>126.58791885410589</v>
+      </c>
+      <c r="H35" s="20">
+        <f t="shared" si="6"/>
+        <v>381.40570888065054</v>
+      </c>
+      <c r="I35" s="20">
+        <f t="shared" si="7"/>
+        <v>841.74233930296998</v>
+      </c>
+      <c r="J35" s="20">
+        <f t="shared" si="8"/>
+        <v>385.00931578165699</v>
+      </c>
+      <c r="K35" s="20">
+        <f t="shared" si="9"/>
+        <v>874.36299923121635</v>
+      </c>
+      <c r="L35" s="20">
+        <f t="shared" si="10"/>
+        <v>384.15598032929262</v>
+      </c>
+      <c r="M35" s="20">
+        <f t="shared" si="11"/>
+        <v>871.90282794799191</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E36" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" s="20">
+        <f t="shared" si="4"/>
+        <v>46.477109465862746</v>
+      </c>
+      <c r="G36" s="20">
+        <f t="shared" si="5"/>
+        <v>43.108323975953141</v>
+      </c>
+      <c r="H36" s="20">
+        <f t="shared" si="6"/>
+        <v>192.65328265781386</v>
+      </c>
+      <c r="I36" s="20">
+        <f t="shared" si="7"/>
+        <v>182.07971449900768</v>
+      </c>
+      <c r="J36" s="20">
+        <f t="shared" si="8"/>
+        <v>199.65419892745763</v>
+      </c>
+      <c r="K36" s="20">
+        <f t="shared" si="9"/>
+        <v>186.12946043838093</v>
+      </c>
+      <c r="L36" s="20">
+        <f t="shared" si="10"/>
+        <v>199.09861276206118</v>
+      </c>
+      <c r="M36" s="20">
+        <f t="shared" si="11"/>
+        <v>187.40921607434518</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E37" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F37" s="20">
+        <f t="shared" si="4"/>
+        <v>61.120151460624932</v>
+      </c>
+      <c r="G37" s="20">
+        <f t="shared" si="5"/>
+        <v>96.338816681875358</v>
+      </c>
+      <c r="H37" s="20">
+        <f t="shared" si="6"/>
+        <v>261.39362534138007</v>
+      </c>
+      <c r="I37" s="20">
+        <f t="shared" si="7"/>
+        <v>410.79571129277406</v>
+      </c>
+      <c r="J37" s="20">
+        <f t="shared" si="8"/>
+        <v>259.96567023341731</v>
+      </c>
+      <c r="K37" s="20">
+        <f t="shared" si="9"/>
+        <v>406.7056819427354</v>
+      </c>
+      <c r="L37" s="20">
+        <f t="shared" si="10"/>
+        <v>260.26979295665882</v>
+      </c>
+      <c r="M37" s="20">
+        <f t="shared" si="11"/>
+        <v>405.52410578195878</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E38" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="20">
+        <f t="shared" si="4"/>
+        <v>65.141079945302337</v>
+      </c>
+      <c r="G38" s="20">
+        <f t="shared" si="5"/>
+        <v>57.959886194604259</v>
+      </c>
+      <c r="H38" s="20">
+        <f t="shared" si="6"/>
+        <v>278.54842842976683</v>
+      </c>
+      <c r="I38" s="20">
+        <f t="shared" si="7"/>
+        <v>244.23221207952983</v>
+      </c>
+      <c r="J38" s="20">
+        <f t="shared" si="8"/>
+        <v>276.96724467653377</v>
+      </c>
+      <c r="K38" s="20">
+        <f t="shared" si="9"/>
+        <v>252.39633759032358</v>
+      </c>
+      <c r="L38" s="20">
+        <f t="shared" si="10"/>
+        <v>276.15047410046679</v>
+      </c>
+      <c r="M38" s="20">
+        <f t="shared" si="11"/>
+        <v>251.8037700567503</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E39" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="20">
+        <f t="shared" si="4"/>
+        <v>10.821364038997078</v>
+      </c>
+      <c r="G39" s="20">
+        <f t="shared" si="5"/>
+        <v>26.503579891543112</v>
+      </c>
+      <c r="H39" s="20">
+        <f t="shared" si="6"/>
+        <v>47.60553671434203</v>
+      </c>
+      <c r="I39" s="20">
+        <f t="shared" si="7"/>
+        <v>135.07971594356692</v>
+      </c>
+      <c r="J39" s="20">
+        <f t="shared" si="8"/>
+        <v>46.99374106810523</v>
+      </c>
+      <c r="K39" s="20">
+        <f t="shared" si="9"/>
+        <v>125.80524596238679</v>
+      </c>
+      <c r="L39" s="20">
+        <f t="shared" si="10"/>
+        <v>47.342342155357393</v>
+      </c>
+      <c r="M39" s="20">
+        <f t="shared" si="11"/>
+        <v>125.71615424218531</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" s="20">
+        <f t="shared" si="4"/>
+        <v>855.18034043018997</v>
+      </c>
+      <c r="G40" s="20">
+        <f t="shared" si="5"/>
+        <v>1100.1971553302351</v>
+      </c>
+      <c r="H40" s="20">
+        <f t="shared" si="6"/>
+        <v>857.50349861427435</v>
+      </c>
+      <c r="I40" s="20">
+        <f t="shared" si="7"/>
+        <v>1171.3771647050005</v>
+      </c>
+      <c r="J40" s="20">
+        <f t="shared" si="8"/>
+        <v>905.3114395832489</v>
+      </c>
+      <c r="K40" s="20">
+        <f t="shared" si="9"/>
+        <v>1168.0805064446652</v>
+      </c>
+      <c r="L40" s="20">
+        <f t="shared" si="10"/>
+        <v>846.66043607956408</v>
+      </c>
+      <c r="M40" s="20">
+        <f t="shared" si="11"/>
+        <v>1166.2039496487714</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" s="20">
+        <f t="shared" si="4"/>
+        <v>389.99126419568199</v>
+      </c>
+      <c r="G41" s="20">
+        <f t="shared" si="5"/>
+        <v>537.96760143917083</v>
+      </c>
+      <c r="H41" s="20">
+        <f t="shared" si="6"/>
+        <v>415.38037211435255</v>
+      </c>
+      <c r="I41" s="20">
+        <f t="shared" si="7"/>
+        <v>579.56097097326824</v>
+      </c>
+      <c r="J41" s="20">
+        <f t="shared" si="8"/>
+        <v>413.10531159449249</v>
+      </c>
+      <c r="K41" s="20">
+        <f t="shared" si="9"/>
+        <v>575.92348971623824</v>
+      </c>
+      <c r="L41" s="20">
+        <f t="shared" si="10"/>
+        <v>412.31299082386818</v>
+      </c>
+      <c r="M41" s="20">
+        <f t="shared" si="11"/>
+        <v>575.75343204988542</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E42" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F42" s="20">
+        <f t="shared" si="4"/>
+        <v>14.545031417267861</v>
+      </c>
+      <c r="G42" s="20">
+        <f t="shared" si="5"/>
+        <v>181.56887125169223</v>
+      </c>
+      <c r="H42" s="20">
+        <f t="shared" si="6"/>
+        <v>12.515710971983131</v>
+      </c>
+      <c r="I42" s="20">
+        <f t="shared" si="7"/>
+        <v>203.46442953457102</v>
+      </c>
+      <c r="J42" s="20">
+        <f t="shared" si="8"/>
+        <v>12.407597403912487</v>
+      </c>
+      <c r="K42" s="20">
+        <f t="shared" si="9"/>
+        <v>193.95244164910488</v>
+      </c>
+      <c r="L42" s="20">
+        <f t="shared" si="10"/>
+        <v>12.565900274230014</v>
+      </c>
+      <c r="M42" s="20">
+        <f t="shared" si="11"/>
+        <v>202.79159882977012</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E43" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43" s="20">
+        <f t="shared" si="4"/>
+        <v>799.76454931668115</v>
+      </c>
+      <c r="G43" s="20">
+        <f t="shared" si="5"/>
+        <v>1143.2229742088898</v>
+      </c>
+      <c r="H43" s="20">
+        <f t="shared" si="6"/>
+        <v>893.95543095803407</v>
+      </c>
+      <c r="I43" s="20">
+        <f t="shared" si="7"/>
+        <v>1226.5243244304022</v>
+      </c>
+      <c r="J43" s="20">
+        <f t="shared" si="8"/>
+        <v>880.98314194708723</v>
+      </c>
+      <c r="K43" s="20">
+        <f t="shared" si="9"/>
+        <v>1217.8417469452722</v>
+      </c>
+      <c r="L43" s="20">
+        <f t="shared" si="10"/>
+        <v>895.42912341565466</v>
+      </c>
+      <c r="M43" s="20">
+        <f t="shared" si="11"/>
+        <v>1219.3132070561207</v>
+      </c>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D45" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D46" s="41"/>
+      <c r="E46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F46" s="1">
+        <v>467871</v>
+      </c>
+      <c r="G46" s="1">
+        <v>905224</v>
+      </c>
+      <c r="H46" s="1">
+        <v>27688889</v>
+      </c>
+      <c r="I46" s="1">
+        <v>28347256279</v>
+      </c>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47" s="1">
+        <v>325573</v>
+      </c>
+      <c r="G47" s="1">
+        <v>642006</v>
+      </c>
+      <c r="H47" s="1">
+        <v>19337433</v>
+      </c>
+      <c r="I47" s="1">
+        <v>19813662908</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F48" s="1">
+        <v>416389</v>
+      </c>
+      <c r="G48" s="1">
+        <v>762633</v>
+      </c>
+      <c r="H48" s="1">
+        <v>23151129</v>
+      </c>
+      <c r="I48" s="1">
+        <v>24236669408</v>
+      </c>
+    </row>
+    <row r="49" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E49" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F49" s="1">
+        <v>245872</v>
+      </c>
+      <c r="G49" s="1">
+        <v>467775</v>
+      </c>
+      <c r="H49" s="1">
+        <v>13262745</v>
+      </c>
+      <c r="I49" s="1">
+        <v>13519289191</v>
+      </c>
+    </row>
+    <row r="50" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E50" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" s="1">
+        <v>45946</v>
+      </c>
+      <c r="G50" s="1">
+        <v>345899</v>
+      </c>
+      <c r="H50" s="1">
+        <v>11067563</v>
+      </c>
+      <c r="I50" s="1">
+        <v>11415155203</v>
+      </c>
+    </row>
+    <row r="51" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E51" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" s="1">
+        <v>724337</v>
+      </c>
+      <c r="G51" s="1">
+        <v>1250016</v>
+      </c>
+      <c r="H51" s="1">
+        <v>38635284</v>
+      </c>
+      <c r="I51" s="1">
+        <v>39538634572</v>
+      </c>
+    </row>
+    <row r="52" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F52" s="1">
+        <v>4612488</v>
+      </c>
+      <c r="G52" s="1">
+        <v>10222808</v>
+      </c>
+      <c r="H52" s="1">
+        <v>319591894</v>
+      </c>
+      <c r="I52" s="1">
+        <v>328405658363</v>
+      </c>
+    </row>
+    <row r="53" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F53" s="1">
+        <v>114374</v>
+      </c>
+      <c r="G53" s="1">
+        <v>214091</v>
+      </c>
+      <c r="H53" s="1">
+        <v>6895937</v>
+      </c>
+      <c r="I53" s="1">
+        <v>7069066112</v>
+      </c>
+    </row>
+    <row r="54" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="1">
+        <v>73141</v>
+      </c>
+      <c r="G54" s="1">
+        <v>159404</v>
+      </c>
+      <c r="H54" s="1">
+        <v>5199406</v>
+      </c>
+      <c r="I54" s="1">
+        <v>5193637037</v>
+      </c>
+    </row>
+    <row r="55" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E55" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" s="1">
+        <v>53547</v>
+      </c>
+      <c r="G55" s="1">
+        <v>99120</v>
+      </c>
+      <c r="H55" s="1">
+        <v>3064694</v>
+      </c>
+      <c r="I55" s="1">
+        <v>3160653145</v>
+      </c>
+    </row>
+    <row r="56" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E56" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="1">
+        <v>47428</v>
+      </c>
+      <c r="G56" s="1">
+        <v>88113</v>
+      </c>
+      <c r="H56" s="1">
+        <v>2837823</v>
+      </c>
+      <c r="I56" s="1">
+        <v>2906605823</v>
+      </c>
+    </row>
+    <row r="57" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E57" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" s="1">
+        <v>295810</v>
+      </c>
+      <c r="G57" s="1">
+        <v>421117</v>
+      </c>
+      <c r="H57" s="1">
+        <v>11302145</v>
+      </c>
+      <c r="I57" s="1">
+        <v>11610571201</v>
+      </c>
+    </row>
+    <row r="58" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F58" s="1">
+        <v>185079</v>
+      </c>
+      <c r="G58" s="1">
+        <v>330195</v>
+      </c>
+      <c r="H58" s="1">
+        <v>10486435</v>
+      </c>
+      <c r="I58" s="1">
+        <v>10759583722</v>
+      </c>
+    </row>
+    <row r="59" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F59" s="1">
+        <v>246864</v>
+      </c>
+      <c r="G59" s="1">
+        <v>297003</v>
+      </c>
+      <c r="H59" s="1">
+        <v>9149518</v>
+      </c>
+      <c r="I59" s="1">
+        <v>9395542413</v>
+      </c>
+    </row>
+    <row r="60" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E60" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F60" s="1">
+        <v>187530</v>
+      </c>
+      <c r="G60" s="1">
+        <v>327735</v>
+      </c>
+      <c r="H60" s="1">
+        <v>10389359</v>
+      </c>
+      <c r="I60" s="1">
+        <v>10662335639</v>
+      </c>
+    </row>
+    <row r="61" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E61" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F61" s="1">
+        <v>724918</v>
+      </c>
+      <c r="G61" s="1">
+        <v>1373025</v>
+      </c>
+      <c r="H61" s="1">
+        <v>42980837</v>
+      </c>
+      <c r="I61" s="1">
+        <v>43711831102</v>
+      </c>
+    </row>
+    <row r="62" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F62" s="1">
+        <v>336187</v>
+      </c>
+      <c r="G62" s="1">
+        <v>648834</v>
+      </c>
+      <c r="H62" s="1">
+        <v>20034640</v>
+      </c>
+      <c r="I62" s="1">
+        <v>20572719936</v>
+      </c>
+    </row>
+    <row r="63" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E63" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F63" s="1">
+        <v>324376</v>
+      </c>
+      <c r="G63" s="1">
+        <v>608575</v>
+      </c>
+      <c r="H63" s="1">
+        <v>19670244</v>
+      </c>
+      <c r="I63" s="1">
+        <v>20201018591</v>
+      </c>
+    </row>
+    <row r="64" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E64" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F64" s="1">
+        <v>255644</v>
+      </c>
+      <c r="G64" s="1">
+        <v>478206</v>
+      </c>
+      <c r="H64" s="1">
+        <v>15386647</v>
+      </c>
+      <c r="I64" s="1">
+        <v>15737515881</v>
+      </c>
+    </row>
+    <row r="65" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E65" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F65" s="1">
+        <v>539166</v>
+      </c>
+      <c r="G65" s="1">
+        <v>1023616</v>
+      </c>
+      <c r="H65" s="1">
+        <v>31696181</v>
+      </c>
+      <c r="I65" s="1">
+        <v>32533269848</v>
+      </c>
+    </row>
+    <row r="66" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E66" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F66" s="1">
+        <v>239864</v>
+      </c>
+      <c r="G66" s="1">
+        <v>448755</v>
+      </c>
+      <c r="H66" s="1">
+        <v>14442141</v>
+      </c>
+      <c r="I66" s="1">
+        <v>14832493094</v>
+      </c>
+    </row>
+    <row r="67" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E67" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1179086</v>
+      </c>
+      <c r="G67" s="1">
+        <v>1850759</v>
+      </c>
+      <c r="H67" s="1">
+        <v>63590353</v>
+      </c>
+      <c r="I67" s="1">
+        <v>65162667832</v>
+      </c>
+    </row>
+    <row r="68" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E68" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1443903</v>
+      </c>
+      <c r="G68" s="1">
+        <v>2625745</v>
+      </c>
+      <c r="H68" s="1">
+        <v>85117718</v>
+      </c>
+      <c r="I68" s="1">
+        <v>86518744395</v>
+      </c>
+    </row>
+    <row r="69" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E69" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F69" s="1">
+        <v>28404</v>
+      </c>
+      <c r="G69" s="1">
+        <v>213424</v>
+      </c>
+      <c r="H69" s="1">
+        <v>6848843</v>
+      </c>
+      <c r="I69" s="1">
+        <v>7024500305</v>
+      </c>
+    </row>
+    <row r="70" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E70" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F70" s="1">
+        <v>18271</v>
+      </c>
+      <c r="G70" s="1">
+        <v>145772</v>
+      </c>
+      <c r="H70" s="1">
+        <v>4418369</v>
+      </c>
+      <c r="I70" s="1">
+        <v>4837830877</v>
+      </c>
+    </row>
+    <row r="71" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E71" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F71" s="1">
+        <v>58089</v>
+      </c>
+      <c r="G71" s="1">
+        <v>431361</v>
+      </c>
+      <c r="H71" s="1">
+        <v>13890734</v>
+      </c>
+      <c r="I71" s="1">
+        <v>14228312927</v>
+      </c>
+    </row>
+    <row r="72" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E72" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F72" s="1">
+        <v>40065</v>
+      </c>
+      <c r="G72" s="1">
+        <v>300929</v>
+      </c>
+      <c r="H72" s="1">
+        <v>9682761</v>
+      </c>
+      <c r="I72" s="1">
+        <v>9934200695</v>
+      </c>
+    </row>
+    <row r="73" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E73" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F73" s="1">
+        <v>172111</v>
+      </c>
+      <c r="G73" s="1">
+        <v>1228716</v>
+      </c>
+      <c r="H73" s="1">
+        <v>41247225</v>
+      </c>
+      <c r="I73" s="1">
+        <v>40396150764</v>
+      </c>
+    </row>
+    <row r="74" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E74" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F74" s="1">
+        <v>1074250</v>
+      </c>
+      <c r="G74" s="1">
+        <v>9987447</v>
+      </c>
+      <c r="H74" s="1">
+        <v>322383123</v>
+      </c>
+      <c r="I74" s="1">
+        <v>325961523696</v>
+      </c>
+    </row>
+    <row r="75" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E75" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F75" s="1">
+        <v>27335</v>
+      </c>
+      <c r="G75" s="1">
+        <v>203828</v>
+      </c>
+      <c r="H75" s="1">
+        <v>6568998</v>
+      </c>
+      <c r="I75" s="1">
+        <v>6718536265</v>
+      </c>
+    </row>
+    <row r="76" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E76" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F76" s="1">
+        <v>19537</v>
+      </c>
+      <c r="G76" s="1">
+        <v>139828</v>
+      </c>
+      <c r="H76" s="1">
+        <v>4540382</v>
+      </c>
+      <c r="I76" s="1">
+        <v>4574343064</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="F26:M26"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="F3:M3"/>
+    <mergeCell ref="P3:W3"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>